<commit_message>
Add file LSTM_GRU, Update code in file Get_100_sysmbols.py and file Get_Data_100_Symbols.py and Update files in folder DATA
</commit_message>
<xml_diff>
--- a/DATA/ACET_stock_data.xlsx
+++ b/DATA/ACET_stock_data.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1483"/>
+  <dimension ref="A1:G1484"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34562,6 +34562,29 @@
         <v>947500</v>
       </c>
     </row>
+    <row r="1484">
+      <c r="A1484" s="2" t="n">
+        <v>45275</v>
+      </c>
+      <c r="B1484" t="n">
+        <v>1.659999966621399</v>
+      </c>
+      <c r="C1484" t="n">
+        <v>1.659999966621399</v>
+      </c>
+      <c r="D1484" t="n">
+        <v>1.559999942779541</v>
+      </c>
+      <c r="E1484" t="n">
+        <v>1.590000033378601</v>
+      </c>
+      <c r="F1484" t="n">
+        <v>1.590000033378601</v>
+      </c>
+      <c r="G1484" t="n">
+        <v>923600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>